<commit_message>
Corrections to HW 2
</commit_message>
<xml_diff>
--- a/homeworks/CF_HW_2_2021_Ans.xlsx
+++ b/homeworks/CF_HW_2_2021_Ans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmcolon1/Dropbox/Corp Finance/Corp Fin Web/Corporate-Finance/homeworks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA8283D-455F-1648-B55D-2C2720F6973A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F1D109-A803-4340-B138-836C289D4C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27820" yWindow="460" windowWidth="25060" windowHeight="27180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26140" yWindow="460" windowWidth="25060" windowHeight="27180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HW 2 Ans" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="95">
   <si>
     <t>Proportion of Total Value * Time</t>
   </si>
@@ -395,9 +395,6 @@
     <t>10-yr annuity starting today</t>
   </si>
   <si>
-    <t>=PV(rate,nper,pmt,fv,type)  with "type" = 1.  Could also do 9YR annuity + 40K</t>
-  </si>
-  <si>
     <t>Starting next year and growing @ 3%</t>
   </si>
   <si>
@@ -441,6 +438,12 @@
   </si>
   <si>
     <t>=PMT(rate,nper,pv,fv,type) @ 4%  Note: if interest rate drops by 1/3, you have to contribute 50% more.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=PV(rate,nper,pmt,fv,type)  with "type" = 1.  </t>
+  </si>
+  <si>
+    <t>Could also do 9YR annuity + 40K</t>
   </si>
 </sst>
 </file>
@@ -867,7 +870,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="219">
+  <cellXfs count="218">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1344,9 +1347,6 @@
     </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="17" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1675,8 +1675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I180"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A70" zoomScale="114" zoomScaleNormal="170" zoomScalePageLayoutView="154" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="114" zoomScaleNormal="170" zoomScalePageLayoutView="154" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1735,103 +1735,108 @@
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="21"/>
-      <c r="C8" s="214"/>
+      <c r="B8" s="176" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="53">
+        <v>250000</v>
+      </c>
       <c r="D8" s="173"/>
       <c r="E8" s="5"/>
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="176" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="53">
-        <v>250000</v>
-      </c>
+      <c r="B9" s="176"/>
+      <c r="C9" s="53"/>
       <c r="D9" s="173"/>
       <c r="E9" s="5"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B10" s="176"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="173"/>
+      <c r="B10" s="176" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="177">
+        <v>360000</v>
+      </c>
+      <c r="D10" s="173" t="s">
+        <v>76</v>
+      </c>
       <c r="E10" s="5"/>
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="176" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="177">
-        <v>360000</v>
-      </c>
-      <c r="D11" s="173" t="s">
-        <v>76</v>
+      <c r="B11" s="176"/>
+      <c r="C11" s="53">
+        <f>C10/(1+C7)^5</f>
+        <v>282069.41992864525</v>
+      </c>
+      <c r="D11" s="214" t="s">
+        <v>68</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" s="176"/>
-      <c r="C12" s="53">
-        <f>C11/(1+C7)^5</f>
-        <v>282069.41992864525</v>
-      </c>
-      <c r="D12" s="215" t="s">
-        <v>68</v>
-      </c>
+      <c r="C12" s="53"/>
+      <c r="D12" s="214"/>
       <c r="E12" s="5"/>
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="176"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="215"/>
+      <c r="B13" s="176" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="177">
+        <v>22800</v>
+      </c>
+      <c r="D13" s="173" t="s">
+        <v>70</v>
+      </c>
       <c r="E13" s="5"/>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="176" t="s">
-        <v>69</v>
-      </c>
-      <c r="C14" s="177">
-        <v>22800</v>
-      </c>
-      <c r="D14" s="173" t="s">
-        <v>70</v>
+      <c r="B14" s="176"/>
+      <c r="C14" s="142">
+        <f>C13/C7</f>
+        <v>456000</v>
+      </c>
+      <c r="D14" s="214" t="s">
+        <v>71</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" s="176"/>
-      <c r="C15" s="142">
-        <f>C14/C7</f>
-        <v>456000</v>
-      </c>
-      <c r="D15" s="215" t="s">
-        <v>71</v>
-      </c>
+      <c r="C15" s="142"/>
+      <c r="D15" s="214"/>
       <c r="E15" s="5"/>
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="176"/>
-      <c r="C16" s="142"/>
-      <c r="D16" s="215"/>
+      <c r="B16" s="176" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="177">
+        <v>40000</v>
+      </c>
+      <c r="D16" s="173" t="s">
+        <v>77</v>
+      </c>
       <c r="E16" s="5"/>
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="176" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="177">
-        <v>40000</v>
-      </c>
-      <c r="D17" s="173" t="s">
-        <v>77</v>
+      <c r="B17" s="146"/>
+      <c r="C17" s="53">
+        <f>-PV(C7,10,C16,0,1)</f>
+        <v>324312.8670257621</v>
+      </c>
+      <c r="D17" s="215" t="s">
+        <v>93</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="4"/>
@@ -1839,19 +1844,16 @@
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" s="146"/>
       <c r="C18" s="53">
-        <f>-PV(C7,9,C17,0,1)</f>
-        <v>298528.51037705032</v>
-      </c>
-      <c r="D18" s="216" t="s">
-        <v>78</v>
+        <f>-PV(C7,9,C16,0,0) + 40000</f>
+        <v>324312.86702576221</v>
+      </c>
+      <c r="D18" s="215" t="s">
+        <v>94</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="146"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="216"/>
       <c r="E19" s="5"/>
       <c r="F19" s="4"/>
     </row>
@@ -1863,7 +1865,7 @@
         <v>13000</v>
       </c>
       <c r="D20" s="173" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="4"/>
@@ -1892,7 +1894,7 @@
     <row r="23" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="180" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="137" t="s">
@@ -1968,7 +1970,7 @@
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B31" s="95" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C31" s="19"/>
       <c r="D31" s="5"/>
@@ -2071,7 +2073,7 @@
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B41" s="95" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C41" s="19"/>
       <c r="D41" s="5"/>
@@ -2160,7 +2162,7 @@
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B49" s="99" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C49" s="19"/>
       <c r="D49" s="54"/>
@@ -2188,7 +2190,7 @@
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B52" s="95" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C52" s="53"/>
       <c r="D52" s="17"/>
@@ -2228,7 +2230,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="D55" s="77" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E55" s="68"/>
       <c r="F55" s="69"/>
@@ -2271,7 +2273,7 @@
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B59" s="95" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C59" s="53"/>
       <c r="D59" s="17"/>
@@ -2461,7 +2463,7 @@
         <v>-2220.4100388329889</v>
       </c>
       <c r="D75" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E75" s="5"/>
       <c r="F75" s="4"/>
@@ -2488,7 +2490,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D77" s="173" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E77" s="5"/>
       <c r="F77" s="4"/>
@@ -2543,7 +2545,7 @@
         <v>-40731.967104781681</v>
       </c>
       <c r="D83" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E83" s="5"/>
       <c r="F83" s="4"/>
@@ -2558,7 +2560,7 @@
         <v>-26921.576938989787</v>
       </c>
       <c r="D84" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E84" s="5"/>
       <c r="F84" s="4"/>
@@ -2909,7 +2911,7 @@
         <v>1.2034525167274303E-2</v>
       </c>
       <c r="D117" s="159" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E117" s="13"/>
       <c r="F117" s="14"/>
@@ -3289,27 +3291,27 @@
       <c r="G171" s="5"/>
     </row>
     <row r="172" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B172" s="217"/>
-      <c r="C172" s="218"/>
-      <c r="D172" s="218"/>
-      <c r="E172" s="218"/>
-      <c r="F172" s="218"/>
+      <c r="B172" s="216"/>
+      <c r="C172" s="217"/>
+      <c r="D172" s="217"/>
+      <c r="E172" s="217"/>
+      <c r="F172" s="217"/>
       <c r="G172" s="5"/>
     </row>
     <row r="173" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B173" s="218"/>
-      <c r="C173" s="218"/>
-      <c r="D173" s="218"/>
-      <c r="E173" s="218"/>
-      <c r="F173" s="218"/>
+      <c r="B173" s="217"/>
+      <c r="C173" s="217"/>
+      <c r="D173" s="217"/>
+      <c r="E173" s="217"/>
+      <c r="F173" s="217"/>
       <c r="G173" s="5"/>
     </row>
     <row r="174" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B174" s="218"/>
-      <c r="C174" s="218"/>
-      <c r="D174" s="218"/>
-      <c r="E174" s="218"/>
-      <c r="F174" s="218"/>
+      <c r="B174" s="217"/>
+      <c r="C174" s="217"/>
+      <c r="D174" s="217"/>
+      <c r="E174" s="217"/>
+      <c r="F174" s="217"/>
       <c r="G174" s="5"/>
     </row>
     <row r="175" spans="2:7" x14ac:dyDescent="0.2">
@@ -3372,7 +3374,7 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" s="181" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E2" s="183" t="s">
         <v>32</v>
@@ -3826,7 +3828,7 @@
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" s="181" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E24" s="183" t="s">
         <v>32</v>
@@ -4367,7 +4369,7 @@
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B47" s="181" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D47" s="201" t="s">
         <v>32</v>

</xml_diff>